<commit_message>
update trim_vec and fix directory
</commit_message>
<xml_diff>
--- a/data/excel/trim/trim_vec.xlsx
+++ b/data/excel/trim/trim_vec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\might.LAPTOP-3DRL1GPG\Documents\daigojinkaku\data\excel\trim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4260EB1-4708-4E2C-8BBD-3F61447F026F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C7106B-D2D1-4F28-A4B9-B9855005955A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="2655" windowWidth="14160" windowHeight="11430" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9420" yWindow="825" windowWidth="14160" windowHeight="11430" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ifvic" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="8">
   <si>
     <t>syr</t>
     <phoneticPr fontId="2"/>
@@ -51,6 +51,22 @@
   </si>
   <si>
     <t>exr</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bsyr</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bsxr</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>beyr</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bexr</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -125,12 +141,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -486,7 +505,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -694,15 +713,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="F1" sqref="F1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -715,8 +734,20 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -732,8 +763,20 @@
       <c r="E2">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <v>0.32</v>
+      </c>
+      <c r="G2">
+        <v>0.21</v>
+      </c>
+      <c r="H2">
+        <v>0.41</v>
+      </c>
+      <c r="I2">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -749,8 +792,20 @@
       <c r="E3">
         <v>0.49299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>0.32</v>
+      </c>
+      <c r="G3">
+        <v>0.34</v>
+      </c>
+      <c r="H3">
+        <v>0.41</v>
+      </c>
+      <c r="I3">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -766,8 +821,20 @@
       <c r="E4">
         <v>0.61299999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>0.32</v>
+      </c>
+      <c r="G4">
+        <v>0.47</v>
+      </c>
+      <c r="H4">
+        <v>0.41</v>
+      </c>
+      <c r="I4">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -783,8 +850,20 @@
       <c r="E5">
         <v>0.73299999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>0.32</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <v>0.41</v>
+      </c>
+      <c r="I5">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -799,25 +878,38 @@
       </c>
       <c r="E6">
         <v>0.85299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.32</v>
+      </c>
+      <c r="G6">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>0.41</v>
+      </c>
+      <c r="I6">
+        <v>0.78400000000000003</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -830,8 +922,20 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -847,8 +951,20 @@
       <c r="E2">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <v>0.45</v>
+      </c>
+      <c r="G2">
+        <v>0.21</v>
+      </c>
+      <c r="H2">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I2">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -864,8 +980,20 @@
       <c r="E3">
         <v>0.49299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>0.45</v>
+      </c>
+      <c r="G3">
+        <v>0.34</v>
+      </c>
+      <c r="H3">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -881,8 +1009,20 @@
       <c r="E4">
         <v>0.61299999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>0.45</v>
+      </c>
+      <c r="G4">
+        <v>0.47</v>
+      </c>
+      <c r="H4">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -898,8 +1038,20 @@
       <c r="E5">
         <v>0.73299999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>0.45</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -914,6 +1066,18 @@
       </c>
       <c r="E6">
         <v>0.85299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.45</v>
+      </c>
+      <c r="G6">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.78400000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -924,15 +1088,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -945,8 +1109,20 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -962,8 +1138,20 @@
       <c r="E2">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G2">
+        <v>0.21</v>
+      </c>
+      <c r="H2">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I2">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -979,8 +1167,20 @@
       <c r="E3">
         <v>0.49299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G3">
+        <v>0.34</v>
+      </c>
+      <c r="H3">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -996,8 +1196,20 @@
       <c r="E4">
         <v>0.61299999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G4">
+        <v>0.47</v>
+      </c>
+      <c r="H4">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I4">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1013,8 +1225,20 @@
       <c r="E5">
         <v>0.73299999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I5">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1029,6 +1253,18 @@
       </c>
       <c r="E6">
         <v>0.85299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G6">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I6">
+        <v>0.78400000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1039,15 +1275,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1060,8 +1296,20 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1077,8 +1325,20 @@
       <c r="E2">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <v>0.66</v>
+      </c>
+      <c r="G2">
+        <v>0.21</v>
+      </c>
+      <c r="H2">
+        <v>0.73</v>
+      </c>
+      <c r="I2">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1094,8 +1354,20 @@
       <c r="E3">
         <v>0.49299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>0.66</v>
+      </c>
+      <c r="G3">
+        <v>0.34</v>
+      </c>
+      <c r="H3">
+        <v>0.73</v>
+      </c>
+      <c r="I3">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1111,8 +1383,20 @@
       <c r="E4">
         <v>0.61299999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>0.66</v>
+      </c>
+      <c r="G4">
+        <v>0.47</v>
+      </c>
+      <c r="H4">
+        <v>0.73</v>
+      </c>
+      <c r="I4">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1128,8 +1412,20 @@
       <c r="E5">
         <v>0.73299999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>0.66</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <v>0.73</v>
+      </c>
+      <c r="I5">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1144,6 +1440,18 @@
       </c>
       <c r="E6">
         <v>0.85299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.66</v>
+      </c>
+      <c r="G6">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>0.73</v>
+      </c>
+      <c r="I6">
+        <v>0.78400000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1154,15 +1462,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1175,8 +1483,20 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1192,8 +1512,20 @@
       <c r="E2">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G2">
+        <v>0.21</v>
+      </c>
+      <c r="H2">
+        <v>0.84</v>
+      </c>
+      <c r="I2">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1209,8 +1541,20 @@
       <c r="E3">
         <v>0.49299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G3">
+        <v>0.34</v>
+      </c>
+      <c r="H3">
+        <v>0.84</v>
+      </c>
+      <c r="I3">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1226,8 +1570,20 @@
       <c r="E4">
         <v>0.61299999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G4">
+        <v>0.47</v>
+      </c>
+      <c r="H4">
+        <v>0.84</v>
+      </c>
+      <c r="I4">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1243,8 +1599,20 @@
       <c r="E5">
         <v>0.73299999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <v>0.84</v>
+      </c>
+      <c r="I5">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1259,6 +1627,18 @@
       </c>
       <c r="E6">
         <v>0.85299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>0.84</v>
+      </c>
+      <c r="I6">
+        <v>0.78400000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>